<commit_message>
Switched to EPPlus instead of Excel.Interop
</commit_message>
<xml_diff>
--- a/Icris.Excel2Api.Console/bin/Debug/sheets/test.xlsx
+++ b/Icris.Excel2Api.Console/bin/Debug/sheets/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A69871FA-7A2C-4C11-8F61-A0C3049AFED2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5153383B-239E-4E80-BE06-3FCB9AAB5D66}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="Process" sheetId="2" r:id="rId2"/>
+    <sheet name="burp" sheetId="2" r:id="rId2"/>
     <sheet name="Output" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -462,7 +462,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="b">
         <f t="shared" si="0"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,7 @@
       </c>
       <c r="C2">
         <f>Input!D2*Input!D3*2 + Input!D3*Input!D4*2+Input!D2*Input!D4*2</f>
-        <v>384</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -710,7 +710,7 @@
       </c>
       <c r="C3">
         <f>Input!D2*Input!D3*Input!D4</f>
-        <v>512</v>
+        <v>576</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -725,7 +725,7 @@
       </c>
       <c r="C4">
         <f>(Input!D2+Input!D3+Input!D4)*4</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -739,8 +739,8 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <f>VLOOKUP(Input!D5,Process!A2:B5,2)*C3/1000</f>
-        <v>4.0294400000000001</v>
+        <f>((VLOOKUP(Input!D5,burp!A2:B5,2,FALSE))*C3)/1000</f>
+        <v>4.5331200000000003</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Ironed out a few bugs, created 'visible' column.
</commit_message>
<xml_diff>
--- a/Icris.Excel2Api.Console/bin/Debug/sheets/test.xlsx
+++ b/Icris.Excel2Api.Console/bin/Debug/sheets/test.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5153383B-239E-4E80-BE06-3FCB9AAB5D66}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211D54A3-F4FA-4D72-8323-5FC8E28A594A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="burp" sheetId="2" r:id="rId2"/>
+    <sheet name="Process" sheetId="2" r:id="rId2"/>
     <sheet name="Output" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -133,6 +138,9 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>Visible</t>
   </si>
 </sst>
 </file>
@@ -459,21 +467,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.1171875" customWidth="1"/>
+    <col min="9" max="9" width="35.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -493,13 +501,16 @@
         <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -519,11 +530,14 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -544,11 +558,14 @@
         <f>E2</f>
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -559,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="b">
         <f t="shared" si="0"/>
@@ -569,11 +586,14 @@
         <f>E3</f>
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -589,10 +609,13 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>26</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -607,12 +630,15 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="12.5859375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -620,7 +646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -628,7 +654,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -636,7 +662,7 @@
         <v>7.87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -644,7 +670,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -661,18 +687,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1868F97-2EE0-488E-B062-012FB15C2071}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.41015625" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -686,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -695,13 +721,13 @@
       </c>
       <c r="C2">
         <f>Input!D2*Input!D3*2 + Input!D3*Input!D4*2+Input!D2*Input!D4*2</f>
-        <v>416</v>
+        <v>384</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -710,13 +736,13 @@
       </c>
       <c r="C3">
         <f>Input!D2*Input!D3*Input!D4</f>
-        <v>576</v>
+        <v>512</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -725,13 +751,13 @@
       </c>
       <c r="C4">
         <f>(Input!D2+Input!D3+Input!D4)*4</f>
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -739,8 +765,8 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <f>((VLOOKUP(Input!D5,burp!A2:B5,2,FALSE))*C3)/1000</f>
-        <v>4.5331200000000003</v>
+        <f>VLOOKUP(Input!D5,Process!A2:B5,2,FALSE)*C3/1000</f>
+        <v>4.0294400000000001</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>

</xml_diff>